<commit_message>
20140425-0723-DWDT Compiles and runs but  has a closed context issue for teh password strength checking code whne registering
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dib's Documents\Projects\Website Template MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\Dibware.Template.Presentation.Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>As a…</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Frequently Asked Questions (FAQ)</t>
   </si>
   <si>
-    <t>Terms and Conditions (T&amp;C)</t>
-  </si>
-  <si>
     <t>Admin user</t>
   </si>
   <si>
@@ -108,6 +105,116 @@
   </si>
   <si>
     <t>when the effect date is reached this is the version of the terms and conditions that is displayed to all users</t>
+  </si>
+  <si>
+    <t>Dated Terms and Conditions (T&amp;C)</t>
+  </si>
+  <si>
+    <t>When only the T&amp;C for the current date period is displayed to public website users</t>
+  </si>
+  <si>
+    <t>the user is always has the most up to date version of the t&amp;C at hand.</t>
+  </si>
+  <si>
+    <t>Error Page</t>
+  </si>
+  <si>
+    <t>Website User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be able to read a statement explaining that an error has happened </t>
+  </si>
+  <si>
+    <t>not be able to see any technical details of the error</t>
+  </si>
+  <si>
+    <t>can not use this information to agressively attack the website</t>
+  </si>
+  <si>
+    <t>am not confused when the application fails tobehve correctly</t>
+  </si>
+  <si>
+    <t>can pass the information on to the developers</t>
+  </si>
+  <si>
+    <t>be able to view a list of all errors that have happened, with details of when they happened and who they happened to</t>
+  </si>
+  <si>
+    <t>be able to view details on the about page</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>be able to add new notifications that will appear when a user views the website for the first time after the notifcation is created.</t>
+  </si>
+  <si>
+    <t>can deliver important messages to web siet users</t>
+  </si>
+  <si>
+    <t>be able to view the notification when I visit the site</t>
+  </si>
+  <si>
+    <t>be able to view all past notifications</t>
+  </si>
+  <si>
+    <t>I can be kept up to date with current news or new features</t>
+  </si>
+  <si>
+    <t>be able to indicate I have read the notifcation so that it does not appear again</t>
+  </si>
+  <si>
+    <t>only receive each notifcation once</t>
+  </si>
+  <si>
+    <t>I receive only new notifcations that I have not read at the start of each session.</t>
+  </si>
+  <si>
+    <t>I can visit a page with all past notifcations</t>
+  </si>
+  <si>
+    <t>so if I need to re-read a notificatio, I can</t>
+  </si>
+  <si>
+    <t>DBA</t>
+  </si>
+  <si>
+    <t>be sure that the smallest amount of disk space is used so we only store state of the relationship that a useer has NOT read a message</t>
+  </si>
+  <si>
+    <t>So that data can be kept to a minimum</t>
+  </si>
+  <si>
+    <t>once a user has read the notifcation once the link record is removed.</t>
+  </si>
+  <si>
+    <t>be able to understand the importance of the notification by the colour</t>
+  </si>
+  <si>
+    <t>can instantly see if it is something I must take note of</t>
+  </si>
+  <si>
+    <t>Important notifications appear red
+Information notifications appear blue
+Other notifcations appear amber</t>
+  </si>
+  <si>
+    <t>so that I can provide "importance" to the notification information</t>
+  </si>
+  <si>
+    <t>be able to set the importance level of a notification</t>
+  </si>
+  <si>
+    <t>I can set the importance level when creating or editing a warning</t>
+  </si>
+  <si>
+    <t>Adin user</t>
+  </si>
+  <si>
+    <t>so that warnings can be created iin advance and only displayed when needed</t>
+  </si>
+  <si>
+    <t>be able to set an effective date for a warning</t>
   </si>
 </sst>
 </file>
@@ -472,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,134 +634,334 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="D27" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="B34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>12</v>
+      <c r="B36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>